<commit_message>
Changed degraders list v2
</commit_message>
<xml_diff>
--- a/Degraders_list_v2.xlsx
+++ b/Degraders_list_v2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9576" uniqueCount="1107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9576" uniqueCount="1106">
   <si>
     <t xml:space="preserve">Microorganism</t>
   </si>
@@ -2059,7 +2059,7 @@
     <t xml:space="preserve">Jarerat, A., Pranamuda, H., &amp; Tokiwa, Y. (2002). Poly (L‐lactide)‐degrading activity in various actinomycetes. Macromolecular Bioscience, 2(9), 420-428.</t>
   </si>
   <si>
-    <t xml:space="preserve"> LACTY 1012 (number-average molecular weight, Mn ¼ 3.4 _x005F_x0001_ 105 ; weight-average molecular weight, Mw¼ 6.5 _x005F_x0001_ 105 ; polydispersity, Mw/Mn ¼ 1.9)</t>
+    <t xml:space="preserve"> LACTY 1012 (number-average molecular weight, Mn ¼ 3.4 _x005F_x005F_x0001_ 105 ; weight-average molecular weight, Mw¼ 6.5 _x005F_x005F_x0001_ 105 ; polydispersity, Mw/Mn ¼ 1.9)</t>
   </si>
   <si>
     <t xml:space="preserve"> Shimadzu Co. Ltd</t>
@@ -3004,9 +3004,6 @@
     <t xml:space="preserve">India</t>
   </si>
   <si>
-    <t xml:space="preserve">Bacillus sp. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Liu, Y., Deng, Y., Chen, P., Duan, M., Lin, X., &amp; Zhang, Y. (2019). Biodegradation analysis of polyvinyl alcohol during the compost burial course. Journal of basic microbiology, 59(4), 368-374.</t>
   </si>
   <si>
@@ -3166,7 +3163,7 @@
     <t xml:space="preserve">Streptomyces omiyaensis</t>
   </si>
   <si>
-    <t xml:space="preserve">Pseudomonas beteli </t>
+    <t xml:space="preserve">Pseudomonas beteli</t>
   </si>
   <si>
     <t xml:space="preserve">Rhodococcus equi</t>
@@ -3468,8 +3465,8 @@
   </sheetPr>
   <dimension ref="A1:S953"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K937" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M949" activeCellId="0" sqref="M949"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A925" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A934" activeCellId="0" sqref="A934"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38752,7 +38749,7 @@
     </row>
     <row r="890" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A890" s="0" t="s">
-        <v>994</v>
+        <v>51</v>
       </c>
       <c r="B890" s="1" t="n">
         <v>0</v>
@@ -38761,7 +38758,7 @@
         <v>969</v>
       </c>
       <c r="D890" s="2" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="E890" s="3" t="s">
         <v>22</v>
@@ -38779,28 +38776,28 @@
         <v>2019</v>
       </c>
       <c r="J890" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="K890" s="3" t="s">
         <v>996</v>
       </c>
-      <c r="K890" s="3" t="s">
+      <c r="L890" s="3" t="s">
         <v>997</v>
       </c>
-      <c r="L890" s="3" t="s">
+      <c r="M890" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N890" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O890" s="3" t="s">
         <v>998</v>
       </c>
-      <c r="M890" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N890" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O890" s="3" t="s">
+      <c r="P890" s="3" t="s">
         <v>999</v>
       </c>
-      <c r="P890" s="3" t="s">
+      <c r="Q890" s="3" t="s">
         <v>1000</v>
-      </c>
-      <c r="Q890" s="3" t="s">
-        <v>1001</v>
       </c>
       <c r="R890" s="3" t="n">
         <v>1</v>
@@ -38820,7 +38817,7 @@
         <v>969</v>
       </c>
       <c r="D891" s="2" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="E891" s="3" t="s">
         <v>22</v>
@@ -38838,28 +38835,28 @@
         <v>2019</v>
       </c>
       <c r="J891" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="K891" s="3" t="s">
         <v>996</v>
       </c>
-      <c r="K891" s="3" t="s">
+      <c r="L891" s="3" t="s">
         <v>997</v>
       </c>
-      <c r="L891" s="3" t="s">
+      <c r="M891" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N891" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O891" s="3" t="s">
         <v>998</v>
       </c>
-      <c r="M891" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N891" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O891" s="3" t="s">
+      <c r="P891" s="3" t="s">
         <v>999</v>
       </c>
-      <c r="P891" s="3" t="s">
+      <c r="Q891" s="3" t="s">
         <v>1000</v>
-      </c>
-      <c r="Q891" s="3" t="s">
-        <v>1001</v>
       </c>
       <c r="R891" s="3" t="n">
         <v>1</v>
@@ -38879,7 +38876,7 @@
         <v>346</v>
       </c>
       <c r="D892" s="2" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E892" s="3" t="s">
         <v>22</v>
@@ -38897,13 +38894,13 @@
         <v>2013</v>
       </c>
       <c r="J892" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K892" s="3" t="s">
         <v>1003</v>
       </c>
-      <c r="K892" s="3" t="s">
+      <c r="L892" s="3" t="s">
         <v>1004</v>
-      </c>
-      <c r="L892" s="3" t="s">
-        <v>1005</v>
       </c>
       <c r="M892" s="3" t="s">
         <v>23</v>
@@ -38915,10 +38912,10 @@
         <v>653</v>
       </c>
       <c r="P892" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="Q892" s="3" t="s">
         <v>1006</v>
-      </c>
-      <c r="Q892" s="3" t="s">
-        <v>1007</v>
       </c>
       <c r="R892" s="3" t="n">
         <v>1</v>
@@ -38929,7 +38926,7 @@
     </row>
     <row r="893" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A893" s="0" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B893" s="1" t="n">
         <v>0</v>
@@ -38938,7 +38935,7 @@
         <v>346</v>
       </c>
       <c r="D893" s="2" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E893" s="3" t="s">
         <v>22</v>
@@ -38956,13 +38953,13 @@
         <v>2013</v>
       </c>
       <c r="J893" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K893" s="3" t="s">
         <v>1003</v>
       </c>
-      <c r="K893" s="3" t="s">
+      <c r="L893" s="3" t="s">
         <v>1004</v>
-      </c>
-      <c r="L893" s="3" t="s">
-        <v>1005</v>
       </c>
       <c r="M893" s="3" t="s">
         <v>23</v>
@@ -38974,10 +38971,10 @@
         <v>653</v>
       </c>
       <c r="P893" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="Q893" s="3" t="s">
         <v>1006</v>
-      </c>
-      <c r="Q893" s="3" t="s">
-        <v>1007</v>
       </c>
       <c r="R893" s="3" t="n">
         <v>1</v>
@@ -38988,7 +38985,7 @@
     </row>
     <row r="894" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A894" s="0" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B894" s="1" t="n">
         <v>0</v>
@@ -38997,7 +38994,7 @@
         <v>262</v>
       </c>
       <c r="D894" s="2" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="E894" s="3" t="s">
         <v>22</v>
@@ -39015,13 +39012,13 @@
         <v>2007</v>
       </c>
       <c r="J894" s="3" t="s">
+        <v>1010</v>
+      </c>
+      <c r="K894" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="K894" s="3" t="s">
+      <c r="L894" s="3" t="s">
         <v>1012</v>
-      </c>
-      <c r="L894" s="3" t="s">
-        <v>1013</v>
       </c>
       <c r="M894" s="3" t="s">
         <v>23</v>
@@ -39047,7 +39044,7 @@
     </row>
     <row r="895" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A895" s="0" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B895" s="1" t="n">
         <v>0</v>
@@ -39056,7 +39053,7 @@
         <v>808</v>
       </c>
       <c r="D895" s="2" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E895" s="3" t="s">
         <v>22</v>
@@ -39077,10 +39074,10 @@
         <v>552</v>
       </c>
       <c r="K895" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="L895" s="3" t="s">
         <v>1016</v>
-      </c>
-      <c r="L895" s="3" t="s">
-        <v>1017</v>
       </c>
       <c r="M895" s="3" t="s">
         <v>22</v>
@@ -39089,13 +39086,13 @@
         <v>38</v>
       </c>
       <c r="O895" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P895" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="Q895" s="3" t="s">
         <v>1018</v>
-      </c>
-      <c r="P895" s="3" t="s">
-        <v>1000</v>
-      </c>
-      <c r="Q895" s="3" t="s">
-        <v>1019</v>
       </c>
       <c r="R895" s="3" t="n">
         <v>1</v>
@@ -39106,7 +39103,7 @@
     </row>
     <row r="896" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A896" s="0" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B896" s="1" t="n">
         <v>0</v>
@@ -39115,7 +39112,7 @@
         <v>808</v>
       </c>
       <c r="D896" s="2" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E896" s="3" t="s">
         <v>22</v>
@@ -39136,10 +39133,10 @@
         <v>552</v>
       </c>
       <c r="K896" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="L896" s="3" t="s">
         <v>1016</v>
-      </c>
-      <c r="L896" s="3" t="s">
-        <v>1017</v>
       </c>
       <c r="M896" s="3" t="s">
         <v>22</v>
@@ -39148,13 +39145,13 @@
         <v>38</v>
       </c>
       <c r="O896" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P896" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="Q896" s="3" t="s">
         <v>1018</v>
-      </c>
-      <c r="P896" s="3" t="s">
-        <v>1000</v>
-      </c>
-      <c r="Q896" s="3" t="s">
-        <v>1019</v>
       </c>
       <c r="R896" s="3" t="n">
         <v>1</v>
@@ -39165,7 +39162,7 @@
     </row>
     <row r="897" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A897" s="0" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B897" s="1" t="n">
         <v>0</v>
@@ -39174,7 +39171,7 @@
         <v>808</v>
       </c>
       <c r="D897" s="2" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E897" s="3" t="s">
         <v>22</v>
@@ -39195,25 +39192,25 @@
         <v>552</v>
       </c>
       <c r="K897" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="L897" s="3" t="s">
         <v>1016</v>
       </c>
-      <c r="L897" s="3" t="s">
+      <c r="M897" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N897" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O897" s="3" t="s">
         <v>1017</v>
       </c>
-      <c r="M897" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N897" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O897" s="3" t="s">
+      <c r="P897" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="Q897" s="3" t="s">
         <v>1018</v>
-      </c>
-      <c r="P897" s="3" t="s">
-        <v>1000</v>
-      </c>
-      <c r="Q897" s="3" t="s">
-        <v>1019</v>
       </c>
       <c r="R897" s="3" t="n">
         <v>1</v>
@@ -39233,7 +39230,7 @@
         <v>808</v>
       </c>
       <c r="D898" s="2" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E898" s="3" t="s">
         <v>22</v>
@@ -39254,25 +39251,25 @@
         <v>552</v>
       </c>
       <c r="K898" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="L898" s="3" t="s">
         <v>1016</v>
       </c>
-      <c r="L898" s="3" t="s">
+      <c r="M898" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N898" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O898" s="3" t="s">
         <v>1017</v>
       </c>
-      <c r="M898" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N898" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O898" s="3" t="s">
+      <c r="P898" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="Q898" s="3" t="s">
         <v>1018</v>
-      </c>
-      <c r="P898" s="3" t="s">
-        <v>1000</v>
-      </c>
-      <c r="Q898" s="3" t="s">
-        <v>1019</v>
       </c>
       <c r="R898" s="3" t="n">
         <v>1</v>
@@ -39283,7 +39280,7 @@
     </row>
     <row r="899" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A899" s="0" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B899" s="1" t="n">
         <v>0</v>
@@ -39292,7 +39289,7 @@
         <v>808</v>
       </c>
       <c r="D899" s="2" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E899" s="3" t="s">
         <v>22</v>
@@ -39313,25 +39310,25 @@
         <v>552</v>
       </c>
       <c r="K899" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="L899" s="3" t="s">
         <v>1016</v>
       </c>
-      <c r="L899" s="3" t="s">
+      <c r="M899" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N899" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O899" s="3" t="s">
         <v>1017</v>
       </c>
-      <c r="M899" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N899" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O899" s="3" t="s">
+      <c r="P899" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="Q899" s="3" t="s">
         <v>1018</v>
-      </c>
-      <c r="P899" s="3" t="s">
-        <v>1000</v>
-      </c>
-      <c r="Q899" s="3" t="s">
-        <v>1019</v>
       </c>
       <c r="R899" s="3" t="n">
         <v>1</v>
@@ -39351,7 +39348,7 @@
         <v>808</v>
       </c>
       <c r="D900" s="2" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E900" s="3" t="s">
         <v>22</v>
@@ -39372,10 +39369,10 @@
         <v>552</v>
       </c>
       <c r="K900" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="L900" s="3" t="s">
         <v>1016</v>
-      </c>
-      <c r="L900" s="3" t="s">
-        <v>1017</v>
       </c>
       <c r="M900" s="3" t="s">
         <v>22</v>
@@ -39384,13 +39381,13 @@
         <v>38</v>
       </c>
       <c r="O900" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P900" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="Q900" s="3" t="s">
         <v>1018</v>
-      </c>
-      <c r="P900" s="3" t="s">
-        <v>1000</v>
-      </c>
-      <c r="Q900" s="3" t="s">
-        <v>1019</v>
       </c>
       <c r="R900" s="3" t="n">
         <v>1</v>
@@ -39401,7 +39398,7 @@
     </row>
     <row r="901" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A901" s="0" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B901" s="1" t="n">
         <v>0</v>
@@ -39410,7 +39407,7 @@
         <v>808</v>
       </c>
       <c r="D901" s="2" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E901" s="3" t="s">
         <v>22</v>
@@ -39431,25 +39428,25 @@
         <v>552</v>
       </c>
       <c r="K901" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="L901" s="3" t="s">
         <v>1016</v>
       </c>
-      <c r="L901" s="3" t="s">
+      <c r="M901" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N901" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O901" s="3" t="s">
         <v>1017</v>
       </c>
-      <c r="M901" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N901" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O901" s="3" t="s">
+      <c r="P901" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="Q901" s="3" t="s">
         <v>1018</v>
-      </c>
-      <c r="P901" s="3" t="s">
-        <v>1000</v>
-      </c>
-      <c r="Q901" s="3" t="s">
-        <v>1019</v>
       </c>
       <c r="R901" s="3" t="n">
         <v>1</v>
@@ -39460,7 +39457,7 @@
     </row>
     <row r="902" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A902" s="0" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B902" s="1" t="n">
         <v>0</v>
@@ -39469,7 +39466,7 @@
         <v>808</v>
       </c>
       <c r="D902" s="2" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E902" s="3" t="s">
         <v>22</v>
@@ -39490,25 +39487,25 @@
         <v>552</v>
       </c>
       <c r="K902" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="L902" s="3" t="s">
         <v>1016</v>
       </c>
-      <c r="L902" s="3" t="s">
+      <c r="M902" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N902" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O902" s="3" t="s">
         <v>1017</v>
       </c>
-      <c r="M902" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N902" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O902" s="3" t="s">
+      <c r="P902" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="Q902" s="3" t="s">
         <v>1018</v>
-      </c>
-      <c r="P902" s="3" t="s">
-        <v>1000</v>
-      </c>
-      <c r="Q902" s="3" t="s">
-        <v>1019</v>
       </c>
       <c r="R902" s="3" t="n">
         <v>1</v>
@@ -39519,7 +39516,7 @@
     </row>
     <row r="903" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A903" s="0" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B903" s="1" t="n">
         <v>0</v>
@@ -39528,46 +39525,46 @@
         <v>969</v>
       </c>
       <c r="D903" s="2" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E903" s="3" t="s">
         <v>1026</v>
-      </c>
-      <c r="E903" s="3" t="s">
-        <v>1027</v>
       </c>
       <c r="F903" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G903" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H903" s="3" t="s">
         <v>1028</v>
-      </c>
-      <c r="H903" s="3" t="s">
-        <v>1029</v>
       </c>
       <c r="I903" s="3" t="n">
         <v>2018</v>
       </c>
       <c r="J903" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="K903" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="L903" s="3" t="s">
         <v>1030</v>
       </c>
-      <c r="L903" s="3" t="s">
+      <c r="M903" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N903" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O903" s="3" t="s">
         <v>1031</v>
       </c>
-      <c r="M903" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N903" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O903" s="3" t="s">
+      <c r="P903" s="3" t="s">
         <v>1032</v>
       </c>
-      <c r="P903" s="3" t="s">
-        <v>1033</v>
-      </c>
       <c r="Q903" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="R903" s="3" t="n">
         <v>1</v>
@@ -39578,7 +39575,7 @@
     </row>
     <row r="904" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A904" s="0" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B904" s="1" t="n">
         <v>0</v>
@@ -39587,7 +39584,7 @@
         <v>527</v>
       </c>
       <c r="D904" s="2" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="E904" s="3" t="s">
         <v>22</v>
@@ -39623,7 +39620,7 @@
         <v>23</v>
       </c>
       <c r="P904" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="Q904" s="3" t="s">
         <v>23</v>
@@ -39646,7 +39643,7 @@
         <v>172</v>
       </c>
       <c r="D905" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E905" s="3" t="s">
         <v>22</v>
@@ -39667,25 +39664,25 @@
         <v>552</v>
       </c>
       <c r="K905" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="L905" s="3" t="s">
         <v>1038</v>
       </c>
-      <c r="L905" s="3" t="s">
+      <c r="M905" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N905" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O905" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P905" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q905" s="3" t="s">
         <v>1039</v>
-      </c>
-      <c r="M905" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N905" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O905" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P905" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q905" s="3" t="s">
-        <v>1040</v>
       </c>
       <c r="R905" s="3" t="n">
         <v>0</v>
@@ -39705,7 +39702,7 @@
         <v>262</v>
       </c>
       <c r="D906" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E906" s="3" t="s">
         <v>22</v>
@@ -39744,7 +39741,7 @@
         <v>23</v>
       </c>
       <c r="Q906" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R906" s="3" t="n">
         <v>0</v>
@@ -39755,7 +39752,7 @@
     </row>
     <row r="907" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A907" s="0" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B907" s="1" t="n">
         <v>0</v>
@@ -39764,7 +39761,7 @@
         <v>172</v>
       </c>
       <c r="D907" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E907" s="3" t="s">
         <v>22</v>
@@ -39785,25 +39782,25 @@
         <v>552</v>
       </c>
       <c r="K907" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="L907" s="3" t="s">
         <v>1038</v>
       </c>
-      <c r="L907" s="3" t="s">
+      <c r="M907" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N907" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O907" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P907" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q907" s="3" t="s">
         <v>1039</v>
-      </c>
-      <c r="M907" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N907" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O907" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P907" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q907" s="3" t="s">
-        <v>1040</v>
       </c>
       <c r="R907" s="3" t="n">
         <v>0</v>
@@ -39814,7 +39811,7 @@
     </row>
     <row r="908" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A908" s="0" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B908" s="1" t="n">
         <v>0</v>
@@ -39823,7 +39820,7 @@
         <v>177</v>
       </c>
       <c r="D908" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E908" s="3" t="s">
         <v>22</v>
@@ -39847,7 +39844,7 @@
         <v>177</v>
       </c>
       <c r="L908" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="M908" s="3" t="s">
         <v>23</v>
@@ -39862,7 +39859,7 @@
         <v>23</v>
       </c>
       <c r="Q908" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R908" s="3" t="n">
         <v>0</v>
@@ -39873,7 +39870,7 @@
     </row>
     <row r="909" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A909" s="0" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B909" s="1" t="n">
         <v>0</v>
@@ -39882,7 +39879,7 @@
         <v>527</v>
       </c>
       <c r="D909" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E909" s="3" t="s">
         <v>22</v>
@@ -39921,7 +39918,7 @@
         <v>23</v>
       </c>
       <c r="Q909" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R909" s="3" t="n">
         <v>0</v>
@@ -39932,7 +39929,7 @@
     </row>
     <row r="910" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A910" s="0" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B910" s="1" t="n">
         <v>0</v>
@@ -39941,7 +39938,7 @@
         <v>628</v>
       </c>
       <c r="D910" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E910" s="3" t="s">
         <v>22</v>
@@ -39980,7 +39977,7 @@
         <v>23</v>
       </c>
       <c r="Q910" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R910" s="3" t="n">
         <v>0</v>
@@ -39991,7 +39988,7 @@
     </row>
     <row r="911" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A911" s="0" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B911" s="1" t="n">
         <v>0</v>
@@ -40000,10 +39997,10 @@
         <v>172</v>
       </c>
       <c r="D911" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E911" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="F911" s="3" t="s">
         <v>22</v>
@@ -40021,25 +40018,25 @@
         <v>552</v>
       </c>
       <c r="K911" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="L911" s="3" t="s">
         <v>1038</v>
       </c>
-      <c r="L911" s="3" t="s">
+      <c r="M911" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N911" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O911" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P911" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q911" s="3" t="s">
         <v>1039</v>
-      </c>
-      <c r="M911" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N911" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O911" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P911" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q911" s="3" t="s">
-        <v>1040</v>
       </c>
       <c r="R911" s="3" t="n">
         <v>0</v>
@@ -40050,7 +40047,7 @@
     </row>
     <row r="912" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A912" s="0" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B912" s="1" t="n">
         <v>0</v>
@@ -40059,7 +40056,7 @@
         <v>177</v>
       </c>
       <c r="D912" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E912" s="3" t="s">
         <v>22</v>
@@ -40083,7 +40080,7 @@
         <v>177</v>
       </c>
       <c r="L912" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="M912" s="3" t="s">
         <v>23</v>
@@ -40098,7 +40095,7 @@
         <v>23</v>
       </c>
       <c r="Q912" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R912" s="3" t="n">
         <v>0</v>
@@ -40109,7 +40106,7 @@
     </row>
     <row r="913" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A913" s="0" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B913" s="1" t="n">
         <v>0</v>
@@ -40118,7 +40115,7 @@
         <v>527</v>
       </c>
       <c r="D913" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E913" s="3" t="s">
         <v>22</v>
@@ -40157,7 +40154,7 @@
         <v>23</v>
       </c>
       <c r="Q913" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R913" s="3" t="n">
         <v>0</v>
@@ -40168,7 +40165,7 @@
     </row>
     <row r="914" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A914" s="0" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B914" s="1" t="n">
         <v>0</v>
@@ -40177,7 +40174,7 @@
         <v>628</v>
       </c>
       <c r="D914" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E914" s="3" t="s">
         <v>22</v>
@@ -40216,7 +40213,7 @@
         <v>23</v>
       </c>
       <c r="Q914" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R914" s="3" t="n">
         <v>0</v>
@@ -40227,7 +40224,7 @@
     </row>
     <row r="915" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A915" s="0" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B915" s="1" t="n">
         <v>0</v>
@@ -40236,10 +40233,10 @@
         <v>262</v>
       </c>
       <c r="D915" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E915" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="F915" s="3" t="s">
         <v>22</v>
@@ -40275,7 +40272,7 @@
         <v>23</v>
       </c>
       <c r="Q915" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R915" s="3" t="n">
         <v>0</v>
@@ -40295,7 +40292,7 @@
         <v>172</v>
       </c>
       <c r="D916" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E916" s="3" t="s">
         <v>22</v>
@@ -40316,25 +40313,25 @@
         <v>552</v>
       </c>
       <c r="K916" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="L916" s="3" t="s">
         <v>1038</v>
       </c>
-      <c r="L916" s="3" t="s">
+      <c r="M916" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N916" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O916" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P916" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q916" s="3" t="s">
         <v>1039</v>
-      </c>
-      <c r="M916" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N916" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O916" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P916" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q916" s="3" t="s">
-        <v>1040</v>
       </c>
       <c r="R916" s="3" t="n">
         <v>0</v>
@@ -40345,7 +40342,7 @@
     </row>
     <row r="917" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A917" s="0" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B917" s="1" t="n">
         <v>0</v>
@@ -40354,7 +40351,7 @@
         <v>172</v>
       </c>
       <c r="D917" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E917" s="3" t="s">
         <v>22</v>
@@ -40375,25 +40372,25 @@
         <v>552</v>
       </c>
       <c r="K917" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="L917" s="3" t="s">
         <v>1038</v>
       </c>
-      <c r="L917" s="3" t="s">
+      <c r="M917" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N917" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O917" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P917" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q917" s="3" t="s">
         <v>1039</v>
-      </c>
-      <c r="M917" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N917" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O917" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P917" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q917" s="3" t="s">
-        <v>1040</v>
       </c>
       <c r="R917" s="3" t="n">
         <v>0</v>
@@ -40404,7 +40401,7 @@
     </row>
     <row r="918" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A918" s="0" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B918" s="1" t="n">
         <v>0</v>
@@ -40413,7 +40410,7 @@
         <v>177</v>
       </c>
       <c r="D918" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E918" s="3" t="s">
         <v>22</v>
@@ -40437,7 +40434,7 @@
         <v>177</v>
       </c>
       <c r="L918" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="M918" s="3" t="s">
         <v>23</v>
@@ -40452,7 +40449,7 @@
         <v>23</v>
       </c>
       <c r="Q918" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R918" s="3" t="n">
         <v>0</v>
@@ -40463,7 +40460,7 @@
     </row>
     <row r="919" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A919" s="0" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B919" s="1" t="n">
         <v>0</v>
@@ -40472,7 +40469,7 @@
         <v>527</v>
       </c>
       <c r="D919" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E919" s="3" t="s">
         <v>22</v>
@@ -40511,7 +40508,7 @@
         <v>23</v>
       </c>
       <c r="Q919" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R919" s="3" t="n">
         <v>0</v>
@@ -40522,7 +40519,7 @@
     </row>
     <row r="920" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A920" s="0" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B920" s="1" t="n">
         <v>0</v>
@@ -40531,7 +40528,7 @@
         <v>628</v>
       </c>
       <c r="D920" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E920" s="3" t="s">
         <v>22</v>
@@ -40570,7 +40567,7 @@
         <v>23</v>
       </c>
       <c r="Q920" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R920" s="3" t="n">
         <v>0</v>
@@ -40581,7 +40578,7 @@
     </row>
     <row r="921" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A921" s="0" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B921" s="1" t="n">
         <v>0</v>
@@ -40590,7 +40587,7 @@
         <v>262</v>
       </c>
       <c r="D921" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E921" s="3" t="s">
         <v>22</v>
@@ -40629,7 +40626,7 @@
         <v>23</v>
       </c>
       <c r="Q921" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R921" s="3" t="n">
         <v>0</v>
@@ -40640,7 +40637,7 @@
     </row>
     <row r="922" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A922" s="0" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B922" s="1" t="n">
         <v>0</v>
@@ -40649,7 +40646,7 @@
         <v>172</v>
       </c>
       <c r="D922" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E922" s="3" t="s">
         <v>22</v>
@@ -40670,25 +40667,25 @@
         <v>552</v>
       </c>
       <c r="K922" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="L922" s="3" t="s">
         <v>1038</v>
       </c>
-      <c r="L922" s="3" t="s">
+      <c r="M922" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N922" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O922" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P922" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q922" s="3" t="s">
         <v>1039</v>
-      </c>
-      <c r="M922" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N922" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O922" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P922" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q922" s="3" t="s">
-        <v>1040</v>
       </c>
       <c r="R922" s="3" t="n">
         <v>0</v>
@@ -40699,7 +40696,7 @@
     </row>
     <row r="923" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A923" s="0" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B923" s="1" t="n">
         <v>0</v>
@@ -40708,7 +40705,7 @@
         <v>527</v>
       </c>
       <c r="D923" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E923" s="3" t="s">
         <v>22</v>
@@ -40747,7 +40744,7 @@
         <v>23</v>
       </c>
       <c r="Q923" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R923" s="3" t="n">
         <v>0</v>
@@ -40758,7 +40755,7 @@
     </row>
     <row r="924" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A924" s="0" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B924" s="1" t="n">
         <v>0</v>
@@ -40767,7 +40764,7 @@
         <v>628</v>
       </c>
       <c r="D924" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E924" s="3" t="s">
         <v>22</v>
@@ -40806,7 +40803,7 @@
         <v>23</v>
       </c>
       <c r="Q924" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R924" s="3" t="n">
         <v>0</v>
@@ -40817,7 +40814,7 @@
     </row>
     <row r="925" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A925" s="0" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B925" s="1" t="n">
         <v>0</v>
@@ -40826,7 +40823,7 @@
         <v>262</v>
       </c>
       <c r="D925" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E925" s="3" t="s">
         <v>22</v>
@@ -40865,7 +40862,7 @@
         <v>23</v>
       </c>
       <c r="Q925" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R925" s="3" t="n">
         <v>0</v>
@@ -40876,7 +40873,7 @@
     </row>
     <row r="926" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A926" s="0" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B926" s="1" t="n">
         <v>0</v>
@@ -40885,7 +40882,7 @@
         <v>172</v>
       </c>
       <c r="D926" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E926" s="3" t="s">
         <v>22</v>
@@ -40906,25 +40903,25 @@
         <v>552</v>
       </c>
       <c r="K926" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="L926" s="3" t="s">
         <v>1038</v>
       </c>
-      <c r="L926" s="3" t="s">
+      <c r="M926" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N926" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O926" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P926" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q926" s="3" t="s">
         <v>1039</v>
-      </c>
-      <c r="M926" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N926" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O926" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P926" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q926" s="3" t="s">
-        <v>1040</v>
       </c>
       <c r="R926" s="3" t="n">
         <v>0</v>
@@ -40935,7 +40932,7 @@
     </row>
     <row r="927" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A927" s="0" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B927" s="1" t="n">
         <v>0</v>
@@ -40944,7 +40941,7 @@
         <v>177</v>
       </c>
       <c r="D927" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E927" s="3" t="s">
         <v>22</v>
@@ -40968,7 +40965,7 @@
         <v>177</v>
       </c>
       <c r="L927" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="M927" s="3" t="s">
         <v>23</v>
@@ -40983,7 +40980,7 @@
         <v>23</v>
       </c>
       <c r="Q927" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R927" s="3" t="n">
         <v>0</v>
@@ -40994,7 +40991,7 @@
     </row>
     <row r="928" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A928" s="0" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B928" s="1" t="n">
         <v>0</v>
@@ -41003,7 +41000,7 @@
         <v>527</v>
       </c>
       <c r="D928" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E928" s="3" t="s">
         <v>22</v>
@@ -41042,7 +41039,7 @@
         <v>23</v>
       </c>
       <c r="Q928" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R928" s="3" t="n">
         <v>0</v>
@@ -41053,7 +41050,7 @@
     </row>
     <row r="929" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A929" s="0" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B929" s="1" t="n">
         <v>0</v>
@@ -41062,7 +41059,7 @@
         <v>628</v>
       </c>
       <c r="D929" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E929" s="3" t="s">
         <v>22</v>
@@ -41101,7 +41098,7 @@
         <v>23</v>
       </c>
       <c r="Q929" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R929" s="3" t="n">
         <v>0</v>
@@ -41112,7 +41109,7 @@
     </row>
     <row r="930" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A930" s="0" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B930" s="1" t="n">
         <v>0</v>
@@ -41121,7 +41118,7 @@
         <v>262</v>
       </c>
       <c r="D930" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E930" s="3" t="s">
         <v>22</v>
@@ -41160,7 +41157,7 @@
         <v>23</v>
       </c>
       <c r="Q930" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R930" s="3" t="n">
         <v>0</v>
@@ -41171,7 +41168,7 @@
     </row>
     <row r="931" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A931" s="0" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B931" s="1" t="n">
         <v>0</v>
@@ -41180,7 +41177,7 @@
         <v>172</v>
       </c>
       <c r="D931" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E931" s="3" t="s">
         <v>22</v>
@@ -41201,25 +41198,25 @@
         <v>552</v>
       </c>
       <c r="K931" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="L931" s="3" t="s">
         <v>1038</v>
       </c>
-      <c r="L931" s="3" t="s">
+      <c r="M931" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N931" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O931" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P931" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q931" s="3" t="s">
         <v>1039</v>
-      </c>
-      <c r="M931" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N931" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O931" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P931" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q931" s="3" t="s">
-        <v>1040</v>
       </c>
       <c r="R931" s="3" t="n">
         <v>0</v>
@@ -41230,7 +41227,7 @@
     </row>
     <row r="932" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A932" s="0" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B932" s="1" t="n">
         <v>0</v>
@@ -41239,7 +41236,7 @@
         <v>172</v>
       </c>
       <c r="D932" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E932" s="3" t="s">
         <v>22</v>
@@ -41260,25 +41257,25 @@
         <v>552</v>
       </c>
       <c r="K932" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="L932" s="3" t="s">
         <v>1038</v>
       </c>
-      <c r="L932" s="3" t="s">
+      <c r="M932" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N932" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O932" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P932" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q932" s="3" t="s">
         <v>1039</v>
-      </c>
-      <c r="M932" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N932" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O932" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P932" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q932" s="3" t="s">
-        <v>1040</v>
       </c>
       <c r="R932" s="3" t="n">
         <v>0</v>
@@ -41289,7 +41286,7 @@
     </row>
     <row r="933" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A933" s="0" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B933" s="1" t="n">
         <v>0</v>
@@ -41298,7 +41295,7 @@
         <v>172</v>
       </c>
       <c r="D933" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E933" s="3" t="s">
         <v>22</v>
@@ -41319,25 +41316,25 @@
         <v>552</v>
       </c>
       <c r="K933" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="L933" s="3" t="s">
         <v>1038</v>
       </c>
-      <c r="L933" s="3" t="s">
+      <c r="M933" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N933" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O933" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P933" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q933" s="3" t="s">
         <v>1039</v>
-      </c>
-      <c r="M933" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N933" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O933" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P933" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q933" s="3" t="s">
-        <v>1040</v>
       </c>
       <c r="R933" s="3" t="n">
         <v>0</v>
@@ -41348,7 +41345,7 @@
     </row>
     <row r="934" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A934" s="0" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B934" s="1" t="n">
         <v>0</v>
@@ -41357,7 +41354,7 @@
         <v>527</v>
       </c>
       <c r="D934" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E934" s="3" t="s">
         <v>22</v>
@@ -41396,7 +41393,7 @@
         <v>23</v>
       </c>
       <c r="Q934" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R934" s="3" t="n">
         <v>0</v>
@@ -41407,7 +41404,7 @@
     </row>
     <row r="935" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A935" s="0" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B935" s="1" t="n">
         <v>0</v>
@@ -41416,7 +41413,7 @@
         <v>628</v>
       </c>
       <c r="D935" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E935" s="3" t="s">
         <v>22</v>
@@ -41455,7 +41452,7 @@
         <v>23</v>
       </c>
       <c r="Q935" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R935" s="3" t="n">
         <v>0</v>
@@ -41466,7 +41463,7 @@
     </row>
     <row r="936" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A936" s="0" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B936" s="1" t="n">
         <v>0</v>
@@ -41475,7 +41472,7 @@
         <v>262</v>
       </c>
       <c r="D936" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E936" s="3" t="s">
         <v>22</v>
@@ -41514,7 +41511,7 @@
         <v>23</v>
       </c>
       <c r="Q936" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R936" s="3" t="n">
         <v>0</v>
@@ -41534,7 +41531,7 @@
         <v>172</v>
       </c>
       <c r="D937" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E937" s="3" t="s">
         <v>22</v>
@@ -41555,25 +41552,25 @@
         <v>552</v>
       </c>
       <c r="K937" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="L937" s="3" t="s">
         <v>1038</v>
       </c>
-      <c r="L937" s="3" t="s">
+      <c r="M937" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N937" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O937" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P937" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q937" s="3" t="s">
         <v>1039</v>
-      </c>
-      <c r="M937" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N937" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O937" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P937" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q937" s="3" t="s">
-        <v>1040</v>
       </c>
       <c r="R937" s="3" t="n">
         <v>0</v>
@@ -41584,7 +41581,7 @@
     </row>
     <row r="938" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A938" s="4" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B938" s="1" t="n">
         <v>0</v>
@@ -41593,7 +41590,7 @@
         <v>183</v>
       </c>
       <c r="D938" s="4" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="E938" s="1" t="s">
         <v>237</v>
@@ -41602,22 +41599,22 @@
         <v>38</v>
       </c>
       <c r="G938" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H938" s="1" t="s">
         <v>1053</v>
-      </c>
-      <c r="H938" s="1" t="s">
-        <v>1054</v>
       </c>
       <c r="I938" s="3" t="n">
         <v>2016</v>
       </c>
       <c r="J938" s="6" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="K938" s="6" t="s">
         <v>183</v>
       </c>
       <c r="L938" s="6" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="M938" s="3" t="s">
         <v>38</v>
@@ -41652,7 +41649,7 @@
         <v>527</v>
       </c>
       <c r="D939" s="2" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="E939" s="3" t="s">
         <v>944</v>
@@ -41661,10 +41658,10 @@
         <v>38</v>
       </c>
       <c r="G939" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="H939" s="3" t="s">
         <v>1058</v>
-      </c>
-      <c r="H939" s="3" t="s">
-        <v>1059</v>
       </c>
       <c r="I939" s="3" t="n">
         <v>2014</v>
@@ -41708,10 +41705,10 @@
         <v>0</v>
       </c>
       <c r="C940" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D940" s="2" t="s">
         <v>1060</v>
-      </c>
-      <c r="D940" s="2" t="s">
-        <v>1061</v>
       </c>
       <c r="E940" s="3" t="s">
         <v>22</v>
@@ -41729,13 +41726,13 @@
         <v>2015</v>
       </c>
       <c r="J940" s="6" t="s">
+        <v>1061</v>
+      </c>
+      <c r="K940" s="6" t="s">
         <v>1062</v>
       </c>
-      <c r="K940" s="6" t="s">
+      <c r="L940" s="6" t="s">
         <v>1063</v>
-      </c>
-      <c r="L940" s="6" t="s">
-        <v>1064</v>
       </c>
       <c r="M940" s="3" t="s">
         <v>23</v>
@@ -41761,7 +41758,7 @@
     </row>
     <row r="941" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A941" s="0" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B941" s="1" t="n">
         <v>0</v>
@@ -41770,10 +41767,10 @@
         <v>262</v>
       </c>
       <c r="D941" s="2" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E941" s="3" t="s">
         <v>1066</v>
-      </c>
-      <c r="E941" s="3" t="s">
-        <v>1067</v>
       </c>
       <c r="F941" s="3" t="s">
         <v>22</v>
@@ -41788,10 +41785,10 @@
         <v>2015</v>
       </c>
       <c r="J941" s="6" t="s">
+        <v>1067</v>
+      </c>
+      <c r="K941" s="6" t="s">
         <v>1068</v>
-      </c>
-      <c r="K941" s="6" t="s">
-        <v>1069</v>
       </c>
       <c r="L941" s="3" t="s">
         <v>910</v>
@@ -41809,7 +41806,7 @@
         <v>653</v>
       </c>
       <c r="Q941" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="R941" s="3" t="n">
         <v>1</v>
@@ -41829,7 +41826,7 @@
         <v>969</v>
       </c>
       <c r="D942" s="2" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="E942" s="3" t="s">
         <v>22</v>
@@ -41847,28 +41844,28 @@
         <v>2018</v>
       </c>
       <c r="J942" s="6" t="s">
+        <v>1071</v>
+      </c>
+      <c r="K942" s="6" t="s">
         <v>1072</v>
       </c>
-      <c r="K942" s="6" t="s">
+      <c r="L942" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M942" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N942" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O942" s="3" t="s">
         <v>1073</v>
       </c>
-      <c r="L942" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M942" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N942" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O942" s="3" t="s">
+      <c r="P942" s="3" t="s">
         <v>1074</v>
       </c>
-      <c r="P942" s="3" t="s">
-        <v>1075</v>
-      </c>
       <c r="Q942" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="R942" s="3" t="n">
         <v>1</v>
@@ -41906,25 +41903,25 @@
         <v>2016</v>
       </c>
       <c r="J943" s="6" t="s">
+        <v>1075</v>
+      </c>
+      <c r="K943" s="6" t="s">
         <v>1076</v>
       </c>
-      <c r="K943" s="6" t="s">
+      <c r="L943" s="3" t="s">
         <v>1077</v>
       </c>
-      <c r="L943" s="3" t="s">
+      <c r="M943" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N943" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O943" s="3" t="s">
         <v>1078</v>
       </c>
-      <c r="M943" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N943" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O943" s="3" t="s">
-        <v>1079</v>
-      </c>
       <c r="P943" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="Q943" s="3" t="s">
         <v>959</v>
@@ -41965,25 +41962,25 @@
         <v>2016</v>
       </c>
       <c r="J944" s="6" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="K944" s="6" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="L944" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="M944" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N944" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O944" s="3" t="s">
         <v>1078</v>
       </c>
-      <c r="M944" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N944" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O944" s="3" t="s">
-        <v>1079</v>
-      </c>
       <c r="P944" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="Q944" s="3" t="s">
         <v>959</v>
@@ -41997,7 +41994,7 @@
     </row>
     <row r="945" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A945" s="0" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B945" s="1" t="n">
         <v>0</v>
@@ -42006,7 +42003,7 @@
         <v>183</v>
       </c>
       <c r="D945" s="2" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="E945" s="3" t="s">
         <v>192</v>
@@ -42015,22 +42012,22 @@
         <v>38</v>
       </c>
       <c r="G945" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="H945" s="0" t="s">
         <v>1083</v>
-      </c>
-      <c r="H945" s="0" t="s">
-        <v>1084</v>
       </c>
       <c r="I945" s="3" t="n">
         <v>2016</v>
       </c>
       <c r="J945" s="6" t="s">
+        <v>1084</v>
+      </c>
+      <c r="K945" s="6" t="s">
         <v>1085</v>
       </c>
-      <c r="K945" s="6" t="s">
+      <c r="L945" s="3" t="s">
         <v>1086</v>
-      </c>
-      <c r="L945" s="3" t="s">
-        <v>1087</v>
       </c>
       <c r="M945" s="3" t="s">
         <v>38</v>
@@ -42062,10 +42059,10 @@
         <v>0</v>
       </c>
       <c r="C946" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D946" s="2" t="s">
         <v>1088</v>
-      </c>
-      <c r="D946" s="2" t="s">
-        <v>1089</v>
       </c>
       <c r="E946" s="3" t="s">
         <v>22</v>
@@ -42083,13 +42080,13 @@
         <v>2017</v>
       </c>
       <c r="J946" s="6" t="s">
+        <v>1089</v>
+      </c>
+      <c r="K946" s="6" t="s">
         <v>1090</v>
       </c>
-      <c r="K946" s="6" t="s">
+      <c r="L946" s="3" t="s">
         <v>1091</v>
-      </c>
-      <c r="L946" s="3" t="s">
-        <v>1092</v>
       </c>
       <c r="M946" s="3" t="s">
         <v>38</v>
@@ -42115,7 +42112,7 @@
     </row>
     <row r="947" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A947" s="0" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B947" s="1" t="n">
         <v>0</v>
@@ -42124,7 +42121,7 @@
         <v>969</v>
       </c>
       <c r="D947" s="2" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E947" s="3" t="s">
         <v>22</v>
@@ -42142,13 +42139,13 @@
         <v>2013</v>
       </c>
       <c r="J947" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="K947" s="6" t="s">
         <v>1095</v>
       </c>
-      <c r="K947" s="6" t="s">
+      <c r="L947" s="3" t="s">
         <v>1096</v>
-      </c>
-      <c r="L947" s="3" t="s">
-        <v>1097</v>
       </c>
       <c r="M947" s="3" t="s">
         <v>38</v>
@@ -42174,7 +42171,7 @@
     </row>
     <row r="948" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A948" s="0" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B948" s="1" t="n">
         <v>0</v>
@@ -42183,7 +42180,7 @@
         <v>969</v>
       </c>
       <c r="D948" s="2" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="E948" s="3" t="s">
         <v>22</v>
@@ -42201,13 +42198,13 @@
         <v>2011</v>
       </c>
       <c r="J948" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="K948" s="6" t="s">
         <v>1100</v>
       </c>
-      <c r="K948" s="6" t="s">
+      <c r="L948" s="3" t="s">
         <v>1101</v>
-      </c>
-      <c r="L948" s="3" t="s">
-        <v>1102</v>
       </c>
       <c r="M948" s="3" t="s">
         <v>38</v>
@@ -42242,7 +42239,7 @@
         <v>969</v>
       </c>
       <c r="D949" s="2" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E949" s="3" t="s">
         <v>22</v>
@@ -42260,13 +42257,13 @@
         <v>2002</v>
       </c>
       <c r="J949" s="6" t="s">
+        <v>1103</v>
+      </c>
+      <c r="K949" s="6" t="s">
         <v>1104</v>
       </c>
-      <c r="K949" s="6" t="s">
+      <c r="L949" s="3" t="s">
         <v>1105</v>
-      </c>
-      <c r="L949" s="3" t="s">
-        <v>1106</v>
       </c>
       <c r="M949" s="3" t="s">
         <v>22</v>

</xml_diff>